<commit_message>
adding chart for surface and price colomns
</commit_message>
<xml_diff>
--- a/output_appart.xlsx
+++ b/output_appart.xlsx
@@ -88,6 +88,1409 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1281</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1281</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1711</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5910</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>912</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4321</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>7135</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>4721</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>7118</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>7165</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>933</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4144</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>913</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>7018</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>6115</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>7165</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>4112</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>9113</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2871</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>6154</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>7108</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>6115</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>7615</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>4112</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>9113</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7018</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>6115</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>7615</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>4112</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>9113</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1231</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>917</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>817</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>923</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>917</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3211</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>987</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6541</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>987</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>9187</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>7541</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>957</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>957</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>6110</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>5111</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>9157</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>7114</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>817</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>817</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>6110</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>5111</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>9157</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>7114</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>6110</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>5111</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>9157</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>7114</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2643,5 +4046,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>